<commit_message>
create duplicated fish id excel, create subset of graphable data, quick plots of all numeric values, need to facet wrap by the beh group
</commit_message>
<xml_diff>
--- a/QC/Duplicated_FishIDs.xlsx
+++ b/QC/Duplicated_FishIDs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t xml:space="preserve">fish_id</t>
   </si>
@@ -56,33 +56,36 @@
     <t xml:space="preserve">thigmotaxis_index</t>
   </si>
   <si>
+    <t xml:space="preserve">entry_to_dark_number_center_point_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entry_to_light_number_center_point_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ave_duration_dark_entry_cum_duration_frequency_seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ave_duration_light_entry_cum_duration_frequency_seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latency_to_enter_dark_latency_to_first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latency_to_enter_light_latency_to_first</t>
+  </si>
+  <si>
     <t xml:space="preserve">beh_flexibility_index_ci_last_30s_ci_first_30s</t>
   </si>
   <si>
+    <t xml:space="preserve">variance_of_ci_during_test_period</t>
+  </si>
+  <si>
     <t xml:space="preserve">speed_in_dark_center_point_mean</t>
   </si>
   <si>
     <t xml:space="preserve">speed_in_light_center_point_mean</t>
   </si>
   <si>
-    <t xml:space="preserve">entry_to_dark_number_center_point_frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entry_to_light_number_center_point_frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ave_duration_dark_entry_cum_duration_frequency_seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ave_duration_light_entry_cum_duration_frequency_seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latency_to_enter_dark_latency_to_first</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latency_to_enter_light_latency_to_first</t>
-  </si>
-  <si>
     <t xml:space="preserve">body_length</t>
   </si>
   <si>
@@ -110,87 +113,90 @@
     <t xml:space="preserve">20191209-Plate1</t>
   </si>
   <si>
+    <t xml:space="preserve">7D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20191204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20191210-20191211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-F11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.7922109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.8951833703849235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5895094696969694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.140913419913417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0260065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.025024499999999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0185175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0943424999999998</t>
+  </si>
+  <si>
     <t xml:space="preserve">7E</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0191204E7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20191210-20191211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-11F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-11M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.7922109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.8951833703849235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0185175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0943424999999998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.5895094696969694</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.140913419913417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0260065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.025024499999999998</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.1737483</t>
   </si>
   <si>
     <t xml:space="preserve">-0.7684651771648021</t>
   </si>
   <si>
+    <t xml:space="preserve">17.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.273966975732602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.283397683295807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8101055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2252205</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.5896925</t>
   </si>
   <si>
     <t xml:space="preserve">4.2498949999999995</t>
   </si>
   <si>
-    <t xml:space="preserve">17.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.273966975732602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.283397683295807</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.8101055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2252205</t>
-  </si>
-  <si>
     <t xml:space="preserve">20191209-Plate2-7E</t>
   </si>
   <si>
@@ -200,10 +206,10 @@
     <t xml:space="preserve">23.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-23F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-23M</t>
+    <t xml:space="preserve">Z2622-F23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M23</t>
   </si>
   <si>
     <t xml:space="preserve">-0.7850854</t>
@@ -212,73 +218,73 @@
     <t xml:space="preserve">-0.4895432789347838</t>
   </si>
   <si>
+    <t xml:space="preserve">13.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.8223279057017545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.873244977081743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5765425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0083415</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.403245</t>
   </si>
   <si>
     <t xml:space="preserve">3.5950325000000003</t>
   </si>
   <si>
-    <t xml:space="preserve">13.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8223279057017545</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.873244977081743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5765425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0083415</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.5833393</t>
   </si>
   <si>
     <t xml:space="preserve">-0.6812599330575241</t>
   </si>
   <si>
+    <t xml:space="preserve">10.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.641228397435897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.617099431818183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2355235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.7607925</t>
   </si>
   <si>
     <t xml:space="preserve">3.3972</t>
   </si>
   <si>
-    <t xml:space="preserve">10.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.641228397435897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.617099431818183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2355235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">20191217-Plate1-7E</t>
   </si>
   <si>
     <t xml:space="preserve">20191217-Plate1</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0191211E7</t>
+    <t xml:space="preserve">20191211</t>
   </si>
   <si>
     <t xml:space="preserve">20191217-20191218</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-13F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-14M</t>
+    <t xml:space="preserve">Z2622-F13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M14</t>
   </si>
   <si>
     <t xml:space="preserve">-0.7701674679898717</t>
@@ -287,57 +293,57 @@
     <t xml:space="preserve">-0.5992566183568613</t>
   </si>
   <si>
+    <t xml:space="preserve">5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.077417476190476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.60746381410257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3336595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6923455000000001</t>
+  </si>
+  <si>
     <t xml:space="preserve">14.96025</t>
   </si>
   <si>
     <t xml:space="preserve">3.32417</t>
   </si>
   <si>
-    <t xml:space="preserve">5.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.077417476190476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44.60746381410257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3336595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6923455000000001</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.14866509375361225</t>
   </si>
   <si>
     <t xml:space="preserve">-0.5068984113169646</t>
   </si>
   <si>
+    <t xml:space="preserve">18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.276288662439613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.41078004104813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.533855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7183475000000001</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.0379375</t>
   </si>
   <si>
     <t xml:space="preserve">3.539605</t>
   </si>
   <si>
-    <t xml:space="preserve">18.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.276288662439613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.41078004104813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.533855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7183475000000001</t>
-  </si>
-  <si>
     <t xml:space="preserve">20191217-Plate2-7E</t>
   </si>
   <si>
@@ -347,10 +353,10 @@
     <t xml:space="preserve">25.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-25F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-26M</t>
+    <t xml:space="preserve">Z2622-F25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M26</t>
   </si>
   <si>
     <t xml:space="preserve">-0.7738565431316964</t>
@@ -359,37 +365,37 @@
     <t xml:space="preserve">-0.5101832526884114</t>
   </si>
   <si>
+    <t xml:space="preserve">9.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7313841666666665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.476335087719299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1094185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.350343</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.78661</t>
   </si>
   <si>
     <t xml:space="preserve">3.613225</t>
   </si>
   <si>
-    <t xml:space="preserve">9.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.7313841666666665</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.476335087719299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1094185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.350343</t>
-  </si>
-  <si>
     <t xml:space="preserve">26.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-26F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-27M</t>
+    <t xml:space="preserve">Z2622-F26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M27</t>
   </si>
   <si>
     <t xml:space="preserve">0.4033657018317903</t>
@@ -398,27 +404,27 @@
     <t xml:space="preserve">-0.7267500904989621</t>
   </si>
   <si>
+    <t xml:space="preserve">15.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.32389132518797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.509440346320346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.500489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.751714</t>
+  </si>
+  <si>
     <t xml:space="preserve">7.406345</t>
   </si>
   <si>
     <t xml:space="preserve">6.34577</t>
   </si>
   <si>
-    <t xml:space="preserve">15.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.32389132518797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.509440346320346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.500489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.751714</t>
-  </si>
-  <si>
     <t xml:space="preserve">20200114-Plate1-1A</t>
   </si>
   <si>
@@ -428,7 +434,7 @@
     <t xml:space="preserve">1A</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0200108E7</t>
+    <t xml:space="preserve">20200108</t>
   </si>
   <si>
     <t xml:space="preserve">20200114-20200115</t>
@@ -437,19 +443,19 @@
     <t xml:space="preserve">1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-1F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-3M</t>
+    <t xml:space="preserve">Z2622-F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M3</t>
   </si>
   <si>
     <t xml:space="preserve">17.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-17F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-19M</t>
+    <t xml:space="preserve">Z2622-F17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M19</t>
   </si>
   <si>
     <t xml:space="preserve">20200114-Plate1-1B</t>
@@ -464,10 +470,10 @@
     <t xml:space="preserve">8.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-8F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-10M</t>
+    <t xml:space="preserve">Z2622-F8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M10</t>
   </si>
   <si>
     <t xml:space="preserve">20200114-Plate2-7E</t>
@@ -479,61 +485,10 @@
     <t xml:space="preserve">28.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Z2622-28F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-30M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate1-1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0200115E7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-20200122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate1-1B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate1-7E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate2-7E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200121-Plate2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2622-36</t>
+    <t xml:space="preserve">Z2622-F28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M30</t>
   </si>
   <si>
     <t xml:space="preserve">20200128-Plate1-1A</t>
@@ -542,37 +497,40 @@
     <t xml:space="preserve">20200128-Plate1</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0200122E7</t>
+    <t xml:space="preserve">20200122</t>
   </si>
   <si>
     <t xml:space="preserve">20200128-20200129</t>
   </si>
   <si>
-    <t xml:space="preserve">2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.0</t>
+    <t xml:space="preserve">2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-F2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M21</t>
   </si>
   <si>
     <t xml:space="preserve">20200128-Plate1-1B</t>
   </si>
   <si>
-    <t xml:space="preserve">2.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">20200128-Plate1-7E</t>
   </si>
   <si>
     <t xml:space="preserve">10.0</t>
   </si>
   <si>
-    <t xml:space="preserve">14a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.0</t>
+    <t xml:space="preserve">Z2622-F10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M14a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M15</t>
   </si>
   <si>
     <t xml:space="preserve">20200128-Plate2-7E</t>
@@ -584,7 +542,76 @@
     <t xml:space="preserve">27.0</t>
   </si>
   <si>
-    <t xml:space="preserve">31.0</t>
+    <t xml:space="preserve">Z2622-F27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200204-Plate2-7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200204-Plate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200204-20200205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M33a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200211-Plate1-7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200211-Plate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200211-20200212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200211-Plate2-7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200211-Plate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-F30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200317-Plate1-7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200317-Plate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200317-20200318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2622-M18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200317-Plate2-7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200317-Plate2</t>
   </si>
 </sst>
 </file>
@@ -1001,635 +1028,646 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2"/>
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" t="s">
-        <v>46</v>
-      </c>
-      <c r="V2" t="s">
         <v>47</v>
       </c>
+      <c r="U2"/>
+      <c r="V2"/>
       <c r="W2" t="s">
         <v>48</v>
       </c>
-      <c r="X2"/>
+      <c r="X2" t="s">
+        <v>49</v>
+      </c>
       <c r="Y2"/>
       <c r="Z2"/>
       <c r="AA2"/>
       <c r="AB2"/>
+      <c r="AC2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3"/>
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
+        <v>53</v>
+      </c>
       <c r="P3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="S3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="T3" t="s">
-        <v>55</v>
-      </c>
-      <c r="U3" t="s">
-        <v>56</v>
-      </c>
-      <c r="V3" t="s">
-        <v>57</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="U3"/>
+      <c r="V3"/>
       <c r="W3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X3"/>
+        <v>59</v>
+      </c>
+      <c r="X3" t="s">
+        <v>60</v>
+      </c>
       <c r="Y3"/>
       <c r="Z3"/>
       <c r="AA3"/>
       <c r="AB3"/>
+      <c r="AC3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4"/>
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="T4" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" t="s">
-        <v>71</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="U4"/>
+      <c r="V4"/>
       <c r="W4" t="s">
-        <v>72</v>
-      </c>
-      <c r="X4"/>
+        <v>73</v>
+      </c>
+      <c r="X4" t="s">
+        <v>74</v>
+      </c>
       <c r="Y4"/>
       <c r="Z4"/>
       <c r="AA4"/>
       <c r="AB4"/>
+      <c r="AC4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5"/>
+        <v>76</v>
+      </c>
+      <c r="O5" t="s">
+        <v>77</v>
+      </c>
       <c r="P5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="R5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="T5" t="s">
-        <v>79</v>
-      </c>
-      <c r="U5" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="U5"/>
+      <c r="V5"/>
       <c r="W5" t="s">
-        <v>82</v>
-      </c>
-      <c r="X5"/>
+        <v>83</v>
+      </c>
+      <c r="X5" t="s">
+        <v>84</v>
+      </c>
       <c r="Y5"/>
       <c r="Z5"/>
       <c r="AA5"/>
       <c r="AB5"/>
+      <c r="AC5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N6" t="s">
-        <v>90</v>
-      </c>
-      <c r="O6"/>
+        <v>92</v>
+      </c>
+      <c r="O6" t="s">
+        <v>93</v>
+      </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Q6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="R6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="T6" t="s">
-        <v>95</v>
-      </c>
-      <c r="U6" t="s">
-        <v>96</v>
-      </c>
-      <c r="V6" t="s">
-        <v>97</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="U6"/>
+      <c r="V6"/>
       <c r="W6" t="s">
-        <v>98</v>
-      </c>
-      <c r="X6"/>
+        <v>99</v>
+      </c>
+      <c r="X6" t="s">
+        <v>100</v>
+      </c>
       <c r="Y6"/>
       <c r="Z6"/>
       <c r="AA6"/>
       <c r="AB6"/>
+      <c r="AC6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O7"/>
+        <v>102</v>
+      </c>
+      <c r="O7" t="s">
+        <v>103</v>
+      </c>
       <c r="P7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="R7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S7" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="T7" t="s">
-        <v>104</v>
-      </c>
-      <c r="U7" t="s">
-        <v>105</v>
-      </c>
-      <c r="V7" t="s">
-        <v>106</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="U7"/>
+      <c r="V7"/>
       <c r="W7" t="s">
-        <v>107</v>
-      </c>
-      <c r="X7"/>
+        <v>108</v>
+      </c>
+      <c r="X7" t="s">
+        <v>109</v>
+      </c>
       <c r="Y7"/>
       <c r="Z7"/>
       <c r="AA7"/>
       <c r="AB7"/>
+      <c r="AC7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N8" t="s">
-        <v>114</v>
-      </c>
-      <c r="O8"/>
+        <v>116</v>
+      </c>
+      <c r="O8" t="s">
+        <v>117</v>
+      </c>
       <c r="P8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="S8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="T8" t="s">
-        <v>119</v>
-      </c>
-      <c r="U8" t="s">
-        <v>120</v>
-      </c>
-      <c r="V8" t="s">
-        <v>121</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="U8"/>
+      <c r="V8"/>
       <c r="W8" t="s">
-        <v>122</v>
-      </c>
-      <c r="X8"/>
+        <v>123</v>
+      </c>
+      <c r="X8" t="s">
+        <v>124</v>
+      </c>
       <c r="Y8"/>
       <c r="Z8"/>
       <c r="AA8"/>
       <c r="AB8"/>
+      <c r="AC8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K9" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>128</v>
+      </c>
+      <c r="N9" t="s">
+        <v>129</v>
+      </c>
+      <c r="O9" t="s">
         <v>125</v>
       </c>
-      <c r="L9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M9" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" t="s">
-        <v>127</v>
-      </c>
-      <c r="O9"/>
       <c r="P9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Q9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="R9" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="S9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="T9" t="s">
-        <v>131</v>
-      </c>
-      <c r="U9" t="s">
-        <v>132</v>
-      </c>
-      <c r="V9" t="s">
-        <v>133</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="U9"/>
+      <c r="V9"/>
       <c r="W9" t="s">
-        <v>134</v>
-      </c>
-      <c r="X9"/>
+        <v>135</v>
+      </c>
+      <c r="X9" t="s">
+        <v>136</v>
+      </c>
       <c r="Y9"/>
       <c r="Z9"/>
       <c r="AA9"/>
       <c r="AB9"/>
+      <c r="AC9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10" t="n">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M10"/>
       <c r="N10"/>
@@ -1647,43 +1685,44 @@
       <c r="Z10"/>
       <c r="AA10"/>
       <c r="AB10"/>
+      <c r="AC10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B11" t="n">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M11"/>
       <c r="N11"/>
@@ -1701,43 +1740,44 @@
       <c r="Z11"/>
       <c r="AA11"/>
       <c r="AB11"/>
+      <c r="AC11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M12"/>
       <c r="N12"/>
@@ -1755,43 +1795,44 @@
       <c r="Z12"/>
       <c r="AA12"/>
       <c r="AB12"/>
+      <c r="AC12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" t="s">
         <v>146</v>
       </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>136</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="K13" t="s">
         <v>147</v>
       </c>
-      <c r="G13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H13" t="s">
-        <v>139</v>
-      </c>
-      <c r="I13" t="s">
-        <v>143</v>
-      </c>
-      <c r="J13" t="s">
-        <v>144</v>
-      </c>
-      <c r="K13" t="s">
-        <v>145</v>
-      </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
@@ -1809,43 +1850,44 @@
       <c r="Z13"/>
       <c r="AA13"/>
       <c r="AB13"/>
+      <c r="AC13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
@@ -1863,43 +1905,44 @@
       <c r="Z14"/>
       <c r="AA14"/>
       <c r="AB14"/>
+      <c r="AC14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M15"/>
       <c r="N15"/>
@@ -1917,43 +1960,44 @@
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
+      <c r="AC15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B16" t="n">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K16" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M16"/>
       <c r="N16"/>
@@ -1971,43 +2015,44 @@
       <c r="Z16"/>
       <c r="AA16"/>
       <c r="AB16"/>
+      <c r="AC16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M17"/>
       <c r="N17"/>
@@ -2025,43 +2070,44 @@
       <c r="Z17"/>
       <c r="AA17"/>
       <c r="AB17"/>
+      <c r="AC17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" t="n">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I18" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="J18" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="L18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M18"/>
       <c r="N18"/>
@@ -2079,43 +2125,44 @@
       <c r="Z18"/>
       <c r="AA18"/>
       <c r="AB18"/>
+      <c r="AC18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B19" t="n">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M19"/>
       <c r="N19"/>
@@ -2133,43 +2180,44 @@
       <c r="Z19"/>
       <c r="AA19"/>
       <c r="AB19"/>
+      <c r="AC19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" t="s">
+        <v>161</v>
+      </c>
+      <c r="H20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I20" t="s">
+        <v>163</v>
+      </c>
+      <c r="J20" t="s">
+        <v>164</v>
+      </c>
+      <c r="K20" t="s">
         <v>165</v>
       </c>
-      <c r="B20" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" t="s">
-        <v>158</v>
-      </c>
-      <c r="F20" t="s">
-        <v>147</v>
-      </c>
-      <c r="G20" t="s">
-        <v>159</v>
-      </c>
-      <c r="H20" t="s">
-        <v>160</v>
-      </c>
-      <c r="I20" t="s">
-        <v>140</v>
-      </c>
-      <c r="J20" t="s">
-        <v>161</v>
-      </c>
-      <c r="K20" t="s">
-        <v>162</v>
-      </c>
       <c r="L20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M20"/>
       <c r="N20"/>
@@ -2187,43 +2235,44 @@
       <c r="Z20"/>
       <c r="AA20"/>
       <c r="AB20"/>
+      <c r="AC20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B21" t="n">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G21" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H21" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I21" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M21"/>
       <c r="N21"/>
@@ -2241,43 +2290,44 @@
       <c r="Z21"/>
       <c r="AA21"/>
       <c r="AB21"/>
+      <c r="AC21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B22" t="n">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="J22" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="L22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M22"/>
       <c r="N22"/>
@@ -2295,43 +2345,44 @@
       <c r="Z22"/>
       <c r="AA22"/>
       <c r="AB22"/>
+      <c r="AC22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B23" t="n">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J23" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="K23" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M23"/>
       <c r="N23"/>
@@ -2349,43 +2400,44 @@
       <c r="Z23"/>
       <c r="AA23"/>
       <c r="AB23"/>
+      <c r="AC23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B24" t="n">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I24" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="J24" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="K24" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="L24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M24"/>
       <c r="N24"/>
@@ -2403,43 +2455,44 @@
       <c r="Z24"/>
       <c r="AA24"/>
       <c r="AB24"/>
+      <c r="AC24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B25" t="n">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I25" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="J25" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="K25" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="L25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M25"/>
       <c r="N25"/>
@@ -2457,40 +2510,45 @@
       <c r="Z25"/>
       <c r="AA25"/>
       <c r="AB25"/>
+      <c r="AC25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="G26" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H26" t="s">
-        <v>177</v>
-      </c>
-      <c r="I26"/>
+        <v>181</v>
+      </c>
+      <c r="I26" t="s">
+        <v>156</v>
+      </c>
       <c r="J26" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="K26" t="s">
-        <v>179</v>
-      </c>
-      <c r="L26"/>
+        <v>182</v>
+      </c>
+      <c r="L26" t="s">
+        <v>39</v>
+      </c>
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -2507,42 +2565,45 @@
       <c r="Z26"/>
       <c r="AA26"/>
       <c r="AB26"/>
+      <c r="AC26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B27" t="n">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H27" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I27" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="J27" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="K27" t="s">
-        <v>180</v>
-      </c>
-      <c r="L27"/>
+        <v>182</v>
+      </c>
+      <c r="L27" t="s">
+        <v>39</v>
+      </c>
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
@@ -2559,40 +2620,41 @@
       <c r="Z27"/>
       <c r="AA27"/>
       <c r="AB27"/>
+      <c r="AC27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="F28" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="J28" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="L28"/>
       <c r="M28"/>
@@ -2611,40 +2673,41 @@
       <c r="Z28"/>
       <c r="AA28"/>
       <c r="AB28"/>
+      <c r="AC28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B29" t="n">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="F29" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I29" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="J29" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="K29" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="L29"/>
       <c r="M29"/>
@@ -2663,40 +2726,41 @@
       <c r="Z29"/>
       <c r="AA29"/>
       <c r="AB29"/>
+      <c r="AC29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B30" t="n">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I30" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="J30" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="K30" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="L30"/>
       <c r="M30"/>
@@ -2715,40 +2779,41 @@
       <c r="Z30"/>
       <c r="AA30"/>
       <c r="AB30"/>
+      <c r="AC30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B31" t="n">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="H31" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I31" t="s">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="J31" t="s">
-        <v>35</v>
+        <v>191</v>
       </c>
       <c r="K31" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="L31"/>
       <c r="M31"/>
@@ -2767,40 +2832,41 @@
       <c r="Z31"/>
       <c r="AA31"/>
       <c r="AB31"/>
+      <c r="AC31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B32" t="n">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="I32" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="J32" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="K32" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="L32"/>
       <c r="M32"/>
@@ -2819,40 +2885,41 @@
       <c r="Z32"/>
       <c r="AA32"/>
       <c r="AB32"/>
+      <c r="AC32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B33" t="n">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="I33" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="J33" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="K33" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="L33"/>
       <c r="M33"/>
@@ -2871,6 +2938,113 @@
       <c r="Z33"/>
       <c r="AA33"/>
       <c r="AB33"/>
+      <c r="AC33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>199</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s">
+        <v>195</v>
+      </c>
+      <c r="H34" t="s">
+        <v>196</v>
+      </c>
+      <c r="I34" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" t="s">
+        <v>126</v>
+      </c>
+      <c r="K34" t="s">
+        <v>192</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" t="s">
+        <v>195</v>
+      </c>
+      <c r="H35" t="s">
+        <v>196</v>
+      </c>
+      <c r="I35" t="s">
+        <v>125</v>
+      </c>
+      <c r="J35" t="s">
+        <v>126</v>
+      </c>
+      <c r="K35" t="s">
+        <v>192</v>
+      </c>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>